<commit_message>
Made update on Accessor Repository files and changes path references
</commit_message>
<xml_diff>
--- a/Submissions/TestData.xlsx
+++ b/Submissions/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj\PycharmProjects\Falcon\Submissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CD57D4-9141-4389-A473-1728970A7541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF692CE6-419B-4D2F-9260-25497E56BD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="5844" windowWidth="23256" windowHeight="14016" activeTab="5" xr2:uid="{E61BD633-247E-4C96-8561-C801128B9409}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E61BD633-247E-4C96-8561-C801128B9409}"/>
   </bookViews>
   <sheets>
     <sheet name="Ford1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="197">
   <si>
     <t>#script</t>
   </si>
@@ -652,31 +652,13 @@
     <t>AIG - American International Specialty Lines Company</t>
   </si>
   <si>
-    <t>NEW-000346</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_Login.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_NewSubmission.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_SearchForSubmission.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_UWQuestions.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_Modifiers.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_UnderLyingPolicies.py</t>
-  </si>
-  <si>
-    <t>Submissions\PyScripts\OneShield_Quotations.py</t>
+    <t>Oneshield2</t>
+  </si>
+  <si>
+    <t>NEW-000570</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -3624,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A213A408-78BC-422E-A1DA-910439CF83F9}">
   <dimension ref="A1:AZ24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3805,7 +3787,7 @@
     </row>
     <row r="2" spans="1:52">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3820,15 +3802,15 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
         <v>83</v>
@@ -3845,13 +3827,13 @@
     </row>
     <row r="4" spans="1:52">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>140</v>
@@ -3862,7 +3844,7 @@
     </row>
     <row r="5" spans="1:52">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -3911,7 +3893,7 @@
     </row>
     <row r="6" spans="1:52">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
@@ -4074,13 +4056,13 @@
     </row>
     <row r="7" spans="1:52">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>71</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>98</v>
@@ -4231,7 +4213,7 @@
     </row>
     <row r="8" spans="1:52">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -8862,7 +8844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8754CC8D-BE98-49CC-A7EB-F30B152BC7E9}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Mada changes to work on Mac OS
</commit_message>
<xml_diff>
--- a/Submissions/TestData.xlsx
+++ b/Submissions/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj\PycharmProjects\Falcon\Submissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudhirrayapureddy/OMSMac/Submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F6FA93-D52A-4B2C-9BBF-BAF97843D8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9255E531-7E1B-1640-A6D9-F484817C15CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{E61BD633-247E-4C96-8561-C801128B9409}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{E61BD633-247E-4C96-8561-C801128B9409}"/>
   </bookViews>
   <sheets>
     <sheet name="Ford1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="208">
   <si>
     <t>#script</t>
   </si>
@@ -670,10 +670,28 @@
     <t>00</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Munich Re - Digital Edge Insurance Company</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_Login.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_NewSubmission.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_SearchForSubmission.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_UWQuestions.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_Modifiers.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_UnderLyingPolicies.py</t>
+  </si>
+  <si>
+    <t>PyScripts/OneShield_Quotations.py</t>
   </si>
 </sst>
 </file>
@@ -1908,7 +1926,7 @@
       <sheetName val="Step 2a"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="8">
           <cell r="E8" t="str">
@@ -1930,23 +1948,128 @@
             <v>600000</v>
           </cell>
         </row>
+        <row r="32">
+          <cell r="E32"/>
+        </row>
+        <row r="33">
+          <cell r="E33"/>
+        </row>
         <row r="37">
           <cell r="E37">
             <v>1.05</v>
           </cell>
         </row>
+        <row r="41">
+          <cell r="E41"/>
+        </row>
+        <row r="44">
+          <cell r="E44"/>
+        </row>
+        <row r="48">
+          <cell r="E48"/>
+        </row>
+        <row r="52">
+          <cell r="E52"/>
+        </row>
         <row r="54">
           <cell r="E54">
             <v>1</v>
           </cell>
         </row>
+        <row r="58">
+          <cell r="E58"/>
+        </row>
+        <row r="72">
+          <cell r="E72"/>
+        </row>
+        <row r="81">
+          <cell r="E81"/>
+        </row>
+        <row r="82">
+          <cell r="E82"/>
+        </row>
+        <row r="83">
+          <cell r="E83"/>
+        </row>
+        <row r="84">
+          <cell r="E84"/>
+        </row>
+        <row r="85">
+          <cell r="E85"/>
+        </row>
+        <row r="86">
+          <cell r="E86"/>
+        </row>
+        <row r="87">
+          <cell r="E87"/>
+        </row>
+        <row r="88">
+          <cell r="E88"/>
+        </row>
+        <row r="89">
+          <cell r="E89"/>
+        </row>
+        <row r="90">
+          <cell r="E90"/>
+        </row>
+        <row r="91">
+          <cell r="E91"/>
+        </row>
+        <row r="92">
+          <cell r="E92"/>
+        </row>
+        <row r="93">
+          <cell r="E93"/>
+        </row>
+        <row r="94">
+          <cell r="E94"/>
+        </row>
+        <row r="95">
+          <cell r="E95"/>
+        </row>
+        <row r="96">
+          <cell r="E96"/>
+        </row>
+        <row r="97">
+          <cell r="E97"/>
+        </row>
+        <row r="98">
+          <cell r="E98"/>
+        </row>
+        <row r="99">
+          <cell r="E99"/>
+        </row>
+        <row r="100">
+          <cell r="E100"/>
+        </row>
+        <row r="101">
+          <cell r="E101"/>
+        </row>
+        <row r="102">
+          <cell r="E102"/>
+        </row>
       </sheetData>
       <sheetData sheetId="2">
+        <row r="9">
+          <cell r="C9"/>
+        </row>
+        <row r="10">
+          <cell r="C10"/>
+        </row>
+        <row r="12">
+          <cell r="C12"/>
+        </row>
+        <row r="14">
+          <cell r="C14"/>
+        </row>
         <row r="15">
           <cell r="C15">
             <v>300000</v>
           </cell>
         </row>
+        <row r="17">
+          <cell r="C17"/>
+        </row>
         <row r="19">
           <cell r="C19" t="str">
             <v>XL</v>
@@ -1993,13 +2116,13 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
       <sheetData sheetId="10">
         <row r="16">
           <cell r="B16" t="str">
@@ -2007,14 +2130,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3478,25 +3601,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A213A408-78BC-422E-A1DA-910439CF83F9}">
   <dimension ref="A1:AZ24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="19" max="19" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -3659,7 +3782,7 @@
     </row>
     <row r="2" spans="1:52">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3679,7 +3802,7 @@
     </row>
     <row r="3" spans="1:52">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>202</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -3699,7 +3822,7 @@
     </row>
     <row r="4" spans="1:52">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>203</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -3719,7 +3842,7 @@
     </row>
     <row r="5" spans="1:52">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>204</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -3768,7 +3891,7 @@
     </row>
     <row r="6" spans="1:52">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>205</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>6</v>
@@ -3931,13 +4054,13 @@
     </row>
     <row r="7" spans="1:52">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>206</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>98</v>
@@ -4088,7 +4211,7 @@
     </row>
     <row r="8" spans="1:52">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>207</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
@@ -4368,28 +4491,28 @@
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="7"/>
-    <col min="3" max="3" width="18.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="7"/>
+    <col min="3" max="3" width="18.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="7"/>
+    <col min="5" max="5" width="9.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" style="7" customWidth="1"/>
     <col min="13" max="13" width="20" style="7" customWidth="1"/>
-    <col min="14" max="18" width="9.140625" style="7"/>
-    <col min="19" max="19" width="45.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="29" width="9.140625" style="7"/>
-    <col min="30" max="30" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="38" width="9.140625" style="7"/>
-    <col min="39" max="39" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="7"/>
+    <col min="14" max="18" width="9.1640625" style="7"/>
+    <col min="19" max="19" width="45.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="29" width="9.1640625" style="7"/>
+    <col min="30" max="30" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="38" width="9.1640625" style="7"/>
+    <col min="39" max="39" width="10.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -5257,26 +5380,26 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="7"/>
-    <col min="3" max="3" width="18.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="7"/>
+    <col min="3" max="3" width="18.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="7"/>
+    <col min="5" max="5" width="9.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" style="7" customWidth="1"/>
     <col min="13" max="13" width="20" style="7" customWidth="1"/>
-    <col min="14" max="18" width="9.140625" style="7"/>
-    <col min="19" max="19" width="45.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="29" width="9.140625" style="7"/>
-    <col min="30" max="30" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="7"/>
+    <col min="14" max="18" width="9.1640625" style="7"/>
+    <col min="19" max="19" width="45.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="29" width="9.1640625" style="7"/>
+    <col min="30" max="30" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -6141,26 +6264,26 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="7"/>
-    <col min="3" max="3" width="18.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="7"/>
+    <col min="3" max="3" width="18.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="7"/>
+    <col min="5" max="5" width="9.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5" style="7" customWidth="1"/>
     <col min="13" max="13" width="20" style="7" customWidth="1"/>
-    <col min="14" max="18" width="9.140625" style="7"/>
-    <col min="19" max="19" width="45.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="29" width="9.140625" style="7"/>
-    <col min="30" max="30" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="7"/>
+    <col min="14" max="18" width="9.1640625" style="7"/>
+    <col min="19" max="19" width="45.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="29" width="9.1640625" style="7"/>
+    <col min="30" max="30" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52">
@@ -7016,11 +7139,11 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8710,21 +8833,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8754CC8D-BE98-49CC-A7EB-F30B152BC7E9}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="7"/>
+    <col min="3" max="3" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75">
+    <row r="1" spans="1:14" ht="16">
       <c r="A1" s="36">
         <v>1</v>
       </c>
@@ -8758,7 +8881,7 @@
       <c r="M1" s="36"/>
       <c r="N1" s="36"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="36">
         <v>2</v>
       </c>
@@ -8792,7 +8915,7 @@
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75">
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" s="36">
         <v>3</v>
       </c>
@@ -8826,7 +8949,7 @@
       <c r="M3" s="36"/>
       <c r="N3" s="36"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75">
+    <row r="4" spans="1:14" ht="16">
       <c r="A4" s="36">
         <v>4</v>
       </c>
@@ -9412,7 +9535,7 @@
         <v>98</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>121</v>

</xml_diff>